<commit_message>
updated excel  assignment :enumeration,serialization,deserialization
</commit_message>
<xml_diff>
--- a/Daily Update/Daily Updates.xlsx
+++ b/Daily Update/Daily Updates.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>SQL by Mr.varun</t>
   </si>
@@ -136,6 +136,28 @@
   </si>
   <si>
     <t>servlet(request object)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub query
+(nested subquery) </t>
+  </si>
+  <si>
+    <t>nested subquery
+Exception,assertion</t>
+  </si>
+  <si>
+    <t>serialization
+deserialization
+enumeration</t>
+  </si>
+  <si>
+    <t>cartesian join,inner join</t>
+  </si>
+  <si>
+    <t>subquery</t>
+  </si>
+  <si>
+    <t>servlet(response object)</t>
   </si>
 </sst>
 </file>
@@ -219,18 +241,11 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -239,7 +254,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,120 +562,136 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="18.75" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="22.625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="23.875" customWidth="1"/>
     <col min="5" max="5" width="19.25" customWidth="1"/>
     <col min="6" max="6" width="20.125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21.75" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1"/>
+    <row r="5" spans="1:8" ht="45">
+      <c r="A5" s="9">
+        <v>43956</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1"/>

</xml_diff>